<commit_message>
Ajustes de unificação da análise do problema, conforme orientação do Takai.
</commit_message>
<xml_diff>
--- a/Requisitos/2 - Analise do Problema/3 - Usuário e Stakeholders.xlsx
+++ b/Requisitos/2 - Analise do Problema/3 - Usuário e Stakeholders.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desenvolvimento\Cursos\Pós Graduação Engenharia de SW\TCC\impacta-es13-gcm-grupo03.github.io\Requisitos\2 - Analise do Problema\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,13 +94,6 @@
     <font>
       <sz val="12.1"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,13 +146,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,9 +500,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -532,25 +526,17 @@
     </row>
     <row r="7" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>